<commit_message>
fitur dan target 1 minggu kedepan
</commit_message>
<xml_diff>
--- a/Fitur.xlsx
+++ b/Fitur.xlsx
@@ -5,15 +5,16 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kuliah\Proyek 3 Travelendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12045" windowHeight="5415" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12045" windowHeight="5415" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fitur" sheetId="3" r:id="rId1"/>
     <sheet name="Pembagian Tugas" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="XXX1048576" localSheetId="0">Fitur!#REF!</definedName>
@@ -29,8 +30,46 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>ZARS</author>
+  </authors>
+  <commentList>
+    <comment ref="D17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ZARS:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+lokasi awal
+lokasi acara
+waktu mulai acara
+waktu selesai
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="86">
   <si>
     <t>Teknologi</t>
   </si>
@@ -62,9 +101,6 @@
     <t>Waktu</t>
   </si>
   <si>
-    <t>Scanning</t>
-  </si>
-  <si>
     <t>Validasi</t>
   </si>
   <si>
@@ -95,9 +131,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Umur</t>
-  </si>
-  <si>
     <t>Data diri</t>
   </si>
   <si>
@@ -155,21 +188,12 @@
     <t>Penyaranan Rute</t>
   </si>
   <si>
-    <t>Waktu Makan</t>
-  </si>
-  <si>
     <t>Log Out</t>
   </si>
   <si>
     <t>Log in</t>
   </si>
   <si>
-    <t>Add</t>
-  </si>
-  <si>
-    <t>Delete</t>
-  </si>
-  <si>
     <t>Muhammad Fizikri A</t>
   </si>
   <si>
@@ -257,18 +281,12 @@
     <t>Setting Akun,Log Out</t>
   </si>
   <si>
-    <t>Ambil Waktu darai server</t>
-  </si>
-  <si>
     <t>Tampilkan waktu</t>
   </si>
   <si>
     <t>Daftar Akun</t>
   </si>
   <si>
-    <t>Pemngingat</t>
-  </si>
-  <si>
     <t>Membuat berbagai kemungkinan arah rute dengan berbagai jenis kendaraan lengkap dengan kecepatan rata2 tiap jenis kendaraan</t>
   </si>
   <si>
@@ -294,13 +312,28 @@
   </si>
   <si>
     <t>Akun (Back End)</t>
+  </si>
+  <si>
+    <t>Alamat rumah</t>
+  </si>
+  <si>
+    <t>Tambah</t>
+  </si>
+  <si>
+    <t>Hapus</t>
+  </si>
+  <si>
+    <t>Pengingat</t>
+  </si>
+  <si>
+    <t>Ambil waktu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,14 +355,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="43">
     <border>
@@ -857,45 +916,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -908,15 +934,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
@@ -927,21 +944,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1002,6 +1004,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1315,12 +1373,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,29 +1390,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="39" t="s">
+      <c r="A1" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="38" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="24" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -1362,328 +1420,322 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="63"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="63"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="63"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="63"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="64"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="26" t="s">
+      <c r="D13" s="17"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="59"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="59"/>
+      <c r="B15" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="57"/>
+      <c r="C21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="17" t="s">
+      <c r="D21" s="22"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D22" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="60"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="B27" s="13"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="13"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="33" t="s">
+      <c r="B28" s="19"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="19"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="33"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
+      <c r="B29" s="19"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="33"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="25"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1696,22 +1748,23 @@
     <mergeCell ref="A19:A25"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A3:A9"/>
-    <mergeCell ref="B3:B8"/>
     <mergeCell ref="A10:A18"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B3:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1721,158 +1774,165 @@
     <col min="3" max="3" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="60" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="66"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="66"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="66"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="62" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" s="62" t="s">
+      <c r="D7" s="66"/>
+    </row>
+    <row r="8" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="66"/>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="65"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="46" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="58" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="52" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="46" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C12" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="46" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="61" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1881,4 +1941,16 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>